<commit_message>
- Actualización de lista de bugs
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>id Bug</t>
   </si>
@@ -59,6 +59,84 @@
   </si>
   <si>
     <t>edicion-configurar.aspx</t>
+  </si>
+  <si>
+    <t>Pasos de Configuración de Edición</t>
+  </si>
+  <si>
+    <t>Falta que te seleccione en el menú el paso en el que estas ubicado en la configuración de la Edición</t>
+  </si>
+  <si>
+    <t>Seleccionar Equipos</t>
+  </si>
+  <si>
+    <t>Flor</t>
+  </si>
+  <si>
+    <t>No me debería dejar seleccionar un solo equipo a participar ni dos tampoco. Cantidad mínima es 3</t>
+  </si>
+  <si>
+    <t>Generación de fixture</t>
+  </si>
+  <si>
+    <t>Cuando la cantidad de equipos de un grupo es impar, me cuenta como equipo el LIBRE</t>
+  </si>
+  <si>
+    <t>Agregar una Fase</t>
+  </si>
+  <si>
+    <t>Sino agrega una fase y toca siguiente, me debería informar que debo agregar una fase</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>No me debería permitir acceder a los pasos "Asignar Equipos", "Generar Fase", "Editar Fecha" sino seleccione las preferencias</t>
+  </si>
+  <si>
+    <t>Tipo de Fixture</t>
+  </si>
+  <si>
+    <t>Si selecciono en el combo tipo de fixture: todos contra todos ida y vuelta, me debería guardar TCT ida y vuelta</t>
+  </si>
+  <si>
+    <t>Nombre de los tipos de fixture</t>
+  </si>
+  <si>
+    <t>El nombre todos contra todos debería incluir que se trata tambien de por grupos</t>
+  </si>
+  <si>
+    <t>Arreglar interfaz modificar usuario</t>
+  </si>
+  <si>
+    <t>Mis datos debería estar centralizado, El panel de éxito esta superpuesto con el botón Modificar</t>
+  </si>
+  <si>
+    <t>Pau</t>
+  </si>
+  <si>
+    <t>Agregar el botón Cancelar</t>
+  </si>
+  <si>
+    <t>Limpiar Datos cuando se modifica exitosamente el usuario</t>
+  </si>
+  <si>
+    <t>Limpiar Datos</t>
+  </si>
+  <si>
+    <t>Modificar datos y después poner mis datos de nuevo (Los datos los obtiene de la Session, debería hacer una consulta en la BD )</t>
+  </si>
+  <si>
+    <t>Modificación de datos</t>
+  </si>
+  <si>
+    <t>usuario-modificar.aspx</t>
+  </si>
+  <si>
+    <t>Cuando se seleccionan los equipos que van a participar en la edición que estoy configurando, una vez que agregué una fase y quiero volver a corregir los equipos que juegan, deberían estar seleccionados los que seleccioné antes</t>
+  </si>
+  <si>
+    <t>CORREGIDO</t>
   </si>
 </sst>
 </file>
@@ -67,14 +145,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,8 +164,14 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,37 +288,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -551,7 +636,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,210 +649,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
corregido bug de tipos de fixture
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -288,16 +288,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -306,9 +300,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,8 +312,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,7 +430,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,352 +655,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>9</v>
+      <c r="F11" s="16" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="11">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="11">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="11">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
- actualizacion de bugs: bugs de modificar usuario OK
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -73,9 +73,6 @@
     <t>Flor</t>
   </si>
   <si>
-    <t>No me debería dejar seleccionar un solo equipo a participar ni dos tampoco. Cantidad mínima es 3</t>
-  </si>
-  <si>
     <t>Generación de fixture</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>CORREGIDO</t>
+  </si>
+  <si>
+    <t>No me debería dejar seleccionar un solo equipo a participar. Cantidad mínima es 2</t>
   </si>
 </sst>
 </file>
@@ -288,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,28 +306,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -395,7 +398,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,7 +433,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -641,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,14 +658,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -685,281 +688,281 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="14" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="F7" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="C8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="12" t="s">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F10" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>7</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="12" t="s">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F11" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="14" t="s">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>10</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>11</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="B16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>12</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>13</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>14</v>
-      </c>
-      <c r="B16" s="14" t="s">
+      <c r="E16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>9</v>
+      <c r="F16" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actualizo lista de bugs
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>id Bug</t>
   </si>
@@ -137,13 +137,22 @@
   </si>
   <si>
     <t>No me debería dejar seleccionar un solo equipo a participar. Cantidad mínima es 2</t>
+  </si>
+  <si>
+    <t>Los grupos se guardan con los mismos equipos</t>
+  </si>
+  <si>
+    <t>edicion-fases.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando crea los grupos de equipos, el objeto fases, devuelve grupos con todos equipos iguales :( </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +176,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
@@ -288,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,9 +327,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -324,14 +336,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,14 +676,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -703,27 +721,27 @@
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>9</v>
+      <c r="F3" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -737,13 +755,13 @@
       <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -751,19 +769,19 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -771,19 +789,19 @@
       <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -791,39 +809,39 @@
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>9</v>
+      <c r="F8" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -837,13 +855,13 @@
       <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -851,19 +869,19 @@
       <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -871,19 +889,19 @@
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -897,13 +915,13 @@
       <c r="C13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -911,17 +929,17 @@
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -929,19 +947,19 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -949,29 +967,41 @@
       <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+    <row r="17" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
- Cambios en BD: Cascada en eliminación de fases, grupos, fechas, partidos - Actualización de lista de bugs
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
   <si>
     <t>id Bug</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cuando crea los grupos de equipos, el objeto fases, devuelve grupos con todos equipos iguales :( </t>
+  </si>
+  <si>
+    <t>Método obtenerUltimoTorneoDelUsurio en DAOTorneo: CAMBIAR!!!!</t>
+  </si>
+  <si>
+    <t>Último Torneo del Usuario</t>
+  </si>
+  <si>
+    <t>login.aspx</t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +358,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -662,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,8 +753,8 @@
       <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>9</v>
+      <c r="F4" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1003,13 +1015,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>

</xml_diff>

<commit_message>
. Actualizacion de la lista de bugs
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>id Bug</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>login.aspx</t>
+  </si>
+  <si>
+    <t>Equipos para generar fixture</t>
+  </si>
+  <si>
+    <t>Deberían ser como mínimo 2</t>
+  </si>
+  <si>
+    <t>modificacion de configuracion de edicion</t>
+  </si>
+  <si>
+    <t>cuando se modific la congiuracion de la edicion deberia generar el fixture con los nuevos equipos</t>
   </si>
 </sst>
 </file>
@@ -312,13 +324,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -354,13 +365,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -674,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,300 +709,300 @@
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -999,10 +1010,10 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1011,7 +1022,7 @@
       <c r="E17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1022,7 +1033,7 @@
       <c r="B18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1031,33 +1042,57 @@
       <c r="E18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
- Actualizacion de lista de bugs
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>id Bug</t>
   </si>
@@ -167,6 +167,30 @@
   </si>
   <si>
     <t>cuando se modific la congiuracion de la edicion deberia generar el fixture con los nuevos equipos</t>
+  </si>
+  <si>
+    <t>No se muestran los NO en configurar edicion</t>
+  </si>
+  <si>
+    <t>No en configurar edicion</t>
+  </si>
+  <si>
+    <t>Cambiar flechita de Quitar Todos</t>
+  </si>
+  <si>
+    <t>Quitar Todos</t>
+  </si>
+  <si>
+    <t>Agregar botón Atrás</t>
+  </si>
+  <si>
+    <t>Limpiar Radio Button de Preferencias</t>
+  </si>
+  <si>
+    <t>Cuando Cambio de SI a No, debe limpiar todos los campos</t>
+  </si>
+  <si>
+    <t>Guardar en Sesion el Fixture</t>
   </si>
 </sst>
 </file>
@@ -233,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -309,22 +333,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="6" tint="0.39991454817346722"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="6" tint="0.39991454817346722"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -334,7 +347,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,6 +386,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,310 +719,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="11" t="s">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="B11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>14</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1010,10 +1030,10 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1022,7 +1042,7 @@
       <c r="E17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1033,7 +1053,7 @@
       <c r="B18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1042,7 +1062,7 @@
       <c r="E18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1059,40 +1079,126 @@
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>9</v>
+      <c r="E19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="16" t="s">
+      <c r="E21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <v>20</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>21</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>22</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>23</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
- Actualización de Lista de BUGS.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
   <si>
     <t>id Bug</t>
   </si>
@@ -191,6 +191,27 @@
   </si>
   <si>
     <t>Guardar en Sesion el Fixture</t>
+  </si>
+  <si>
+    <t>Cantidad de Equipos</t>
+  </si>
+  <si>
+    <t>Agregar la cantidad de equipos seleccionados</t>
+  </si>
+  <si>
+    <t>Tamaño del txt en Recuperar contraseña debe ser mas grande</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recuperar contraseña </t>
+  </si>
+  <si>
+    <t>usuario-recuperar.aspx</t>
+  </si>
+  <si>
+    <t>Ver el panel éxito</t>
+  </si>
+  <si>
+    <t>Botón Guardar deberia estar en verde</t>
   </si>
 </sst>
 </file>
@@ -337,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,12 +401,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -394,6 +409,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,14 +746,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -904,8 +931,8 @@
       <c r="E10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>9</v>
+      <c r="F10" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1127,16 +1154,16 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+      <c r="A22" s="16">
         <v>20</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -1147,13 +1174,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="9" t="s">
@@ -1164,16 +1191,16 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="18">
+      <c r="A24" s="16">
         <v>22</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -1184,19 +1211,90 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
+      <c r="A25" s="16">
         <v>23</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="17" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>24</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>25</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>26</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>27</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Subo Avances en el Mnual de Usuario y em informe de Impacto Ambiental
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>id Bug</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>Botón Guardar deberia estar en verde</t>
+  </si>
+  <si>
+    <t>Equipo libre en los equipos de una fase</t>
+  </si>
+  <si>
+    <t>gestorFase</t>
   </si>
 </sst>
 </file>
@@ -409,17 +415,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,14 +752,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1254,10 +1260,10 @@
       <c r="B27" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="21" t="s">
         <v>63</v>
       </c>
       <c r="F27" s="15" t="s">
@@ -1274,7 +1280,7 @@
       <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="21" t="s">
         <v>63</v>
       </c>
       <c r="F28" s="15" t="s">
@@ -1291,11 +1297,28 @@
       <c r="C29" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="21" t="s">
         <v>63</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>28</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Subo Resultados Testing
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -253,7 +253,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
@@ -401,9 +400,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -426,6 +422,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,7 +738,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,14 +751,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1063,7 +1062,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="23" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -1095,7 +1094,7 @@
       <c r="E18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1160,16 +1159,16 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>20</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -1180,13 +1179,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>21</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="9" t="s">
@@ -1197,16 +1196,16 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <v>22</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -1217,104 +1216,104 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>23</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>24</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <v>26</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>27</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <v>28</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="20" t="s">
         <v>67</v>
       </c>
       <c r="F30" s="12" t="s">

</xml_diff>

<commit_message>
- Actualización de BUGS.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -262,10 +262,10 @@
     <t>Buscador en los Combos</t>
   </si>
   <si>
-    <t>Implementar buscador en los cambios</t>
-  </si>
-  <si>
     <t>todos</t>
+  </si>
+  <si>
+    <t>Implementar buscador en los combos</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,16 +1497,16 @@
         <v>81</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>9</v>
+        <v>82</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Subo Casos de Prueba Sprint 8 y 9
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="95">
   <si>
     <t>id Bug</t>
   </si>
@@ -266,6 +266,41 @@
   </si>
   <si>
     <t>Implementar buscador en los combos</t>
+  </si>
+  <si>
+    <t>Error en el asistente de configuración</t>
+  </si>
+  <si>
+    <t>Configurar edicion: configurar preferencias, elegir 8 equipos, agregar una fase y mostrar el fixture, tocar volver, seleccionar 3 equipos, va a salir el cartel que va a modificarse el fixture, poner aceptar, poner siguiente y se produce un error</t>
+  </si>
+  <si>
+    <t>admin/edicion/equipos.aspx</t>
+  </si>
+  <si>
+    <t>INTERFAZ PARTIDOS: Arreglos menores</t>
+  </si>
+  <si>
+    <t>Otros partidos de la fecha: colorcito de los estados
+- Widget versus: cambiar foto Partidos Empatados y Partidos Perdidos</t>
+  </si>
+  <si>
+    <t>torneo/partido</t>
+  </si>
+  <si>
+    <t>Sacar Notificaciones (módulo admin)</t>
+  </si>
+  <si>
+    <t>admin/</t>
+  </si>
+  <si>
+    <t>Colorcito de los Resultados (Empatado - Perdido - Ganado)
+- Me parece que falta PROXIMOS PARTIDOS!</t>
+  </si>
+  <si>
+    <t>INTERFAZ EQUIPOS: Arreglos menores</t>
+  </si>
+  <si>
+    <t>torneo/equipo</t>
   </si>
 </sst>
 </file>
@@ -411,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -469,6 +504,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,19 +833,19 @@
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1425,8 +1463,8 @@
       <c r="E33" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>9</v>
+      <c r="F33" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1509,9 +1547,91 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>36</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>37</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>38</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>39</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subo avances en el product backlog
</commit_message>
<xml_diff>
--- a/Documentacion/Testing/BUGS.xlsx
+++ b/Documentacion/Testing/BUGS.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="103">
   <si>
     <t>id Bug</t>
   </si>
@@ -301,6 +301,30 @@
   </si>
   <si>
     <t>torneo/equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empate de Partidos </t>
+  </si>
+  <si>
+    <t>No permite empates cuando hay dos fases: TCT y eliminatorio</t>
+  </si>
+  <si>
+    <t>admin/fechas.aspx</t>
+  </si>
+  <si>
+    <t>Se rompe el estilo cuando se selecciona la fecha (FECHA ELIMINATORIA)</t>
+  </si>
+  <si>
+    <t>torneo/fechas</t>
+  </si>
+  <si>
+    <t>Filtro de equipos en fixture</t>
+  </si>
+  <si>
+    <t>Que aplique para la fase correcta. Y si es fase eliminatoria Que no aparezca</t>
+  </si>
+  <si>
+    <t>torneo/fixture</t>
   </si>
 </sst>
 </file>
@@ -822,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,14 +1648,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>41</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>42</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>